<commit_message>
Excel Notes wtih graphs info update
</commit_message>
<xml_diff>
--- a/Excel/Excel_Assignment.xlsx
+++ b/Excel/Excel_Assignment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kishan\Desktop\Bootcamp.Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kishan\Desktop\Bootcamp.Info\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3B1839-28B5-418D-8ADE-58473AF90AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF006D01-D46B-429F-B4DB-334878715ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{924E5CF3-0193-4F0E-80BC-71EDB032F5EC}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="136">
   <si>
     <t>Food ID</t>
   </si>
@@ -482,12 +482,6 @@
     <t xml:space="preserve">CusMomer </t>
   </si>
   <si>
-    <t xml:space="preserve">FirsM </t>
-  </si>
-  <si>
-    <t>LasM</t>
-  </si>
-  <si>
     <t>SamanMha</t>
   </si>
   <si>
@@ -525,6 +519,18 @@
   </si>
   <si>
     <t>Customer ID who bought Lettuce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give 10% coupon </t>
+  </si>
+  <si>
+    <t>Sorry bruh you got E coli</t>
+  </si>
+  <si>
+    <t>FirsM Name</t>
+  </si>
+  <si>
+    <t>LasM Name</t>
   </si>
 </sst>
 </file>
@@ -712,6 +718,9 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -742,9 +751,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1470,35 +1476,41 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585768B9-AC05-43AC-9899-2F47AB07A16A}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="21.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="17" t="s">
         <v>82</v>
       </c>
       <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" t="s">
         <v>131</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>27</v>
       </c>
@@ -7450,7 +7462,7 @@
   <dimension ref="A1:W100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7512,16 +7524,16 @@
       <c r="O1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
@@ -7574,14 +7586,14 @@
         <f>MIN(F2:F100)</f>
         <v>1.26</v>
       </c>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
     </row>
     <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
@@ -7615,14 +7627,14 @@
       <c r="I3" t="s">
         <v>113</v>
       </c>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
@@ -7649,14 +7661,14 @@
         <f t="shared" si="2"/>
         <v>38.975999999999999</v>
       </c>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
@@ -7683,14 +7695,14 @@
         <f t="shared" si="2"/>
         <v>146.16</v>
       </c>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
@@ -7717,14 +7729,14 @@
         <f t="shared" si="2"/>
         <v>121.8</v>
       </c>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -7751,14 +7763,14 @@
         <f t="shared" si="2"/>
         <v>32.886000000000003</v>
       </c>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -7785,14 +7797,14 @@
         <f t="shared" si="2"/>
         <v>14.616000000000001</v>
       </c>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
@@ -7819,14 +7831,14 @@
         <f t="shared" si="2"/>
         <v>3.6540000000000004</v>
       </c>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
@@ -7853,14 +7865,14 @@
         <f t="shared" si="2"/>
         <v>10.474799999999998</v>
       </c>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
@@ -7887,14 +7899,14 @@
         <f t="shared" si="2"/>
         <v>1.4616</v>
       </c>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
@@ -7921,14 +7933,14 @@
         <f t="shared" si="2"/>
         <v>109.61999999999999</v>
       </c>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
@@ -7955,14 +7967,14 @@
         <f t="shared" si="2"/>
         <v>5.8464</v>
       </c>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
@@ -7989,14 +8001,14 @@
         <f t="shared" si="2"/>
         <v>9.8048999999999982</v>
       </c>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="16"/>
-      <c r="W14" s="16"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
@@ -10257,14 +10269,14 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10272,10 +10284,10 @@
         <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10283,22 +10295,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="19"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="22"/>
       <c r="X2" s="5"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -10306,20 +10318,20 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="22"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="25"/>
       <c r="X3" s="5"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
@@ -10332,15 +10344,15 @@
       <c r="C4" t="s">
         <v>71</v>
       </c>
-      <c r="O4" s="20"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="22"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="25"/>
       <c r="X4" s="5"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
@@ -10351,17 +10363,17 @@
         <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
-      </c>
-      <c r="O5" s="20"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="22"/>
+        <v>121</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="25"/>
       <c r="X5" s="5"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -10372,17 +10384,17 @@
         <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
-      </c>
-      <c r="O6" s="20"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="22"/>
+        <v>122</v>
+      </c>
+      <c r="O6" s="23"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="25"/>
       <c r="X6" s="5"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -10395,15 +10407,15 @@
       <c r="C7" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="20"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="22"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="25"/>
       <c r="X7" s="5"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
@@ -10411,20 +10423,20 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="O8" s="20"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="22"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="25"/>
       <c r="X8" s="5"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
@@ -10432,20 +10444,20 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
         <v>79</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="22"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="25"/>
       <c r="X9" s="5"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -10458,15 +10470,15 @@
       <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="22"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="25"/>
       <c r="X10" s="5"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -10479,15 +10491,15 @@
       <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="22"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="25"/>
       <c r="X11" s="5"/>
     </row>
     <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10500,15 +10512,15 @@
       <c r="C12" t="s">
         <v>49</v>
       </c>
-      <c r="O12" s="23"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="25"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="28"/>
       <c r="X12" s="5"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
@@ -10519,7 +10531,7 @@
         <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
@@ -10537,7 +10549,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C14" t="s">
         <v>53</v>
@@ -10558,10 +10570,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
@@ -10673,7 +10685,7 @@
   <dimension ref="A1:Z252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10692,14 +10704,14 @@
       <c r="B1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="17" t="s">
         <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10716,21 +10728,21 @@
         <v>26</v>
       </c>
       <c r="E2" s="11">
-        <f>C2*D2*(1+$Z$4)</f>
+        <f t="shared" ref="E2:E21" si="0">C2*D2*(1+$Z$4)</f>
         <v>136.5</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="19"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="22"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
@@ -10746,19 +10758,19 @@
         <v>69</v>
       </c>
       <c r="E3" s="11">
-        <f>C3*D3*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>362.25</v>
       </c>
-      <c r="N3" s="20"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="22"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="25"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
@@ -10774,20 +10786,20 @@
         <v>3</v>
       </c>
       <c r="E4" s="11">
-        <f>C4*D4*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>9.4500000000000011</v>
       </c>
-      <c r="N4" s="20"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="22"/>
-      <c r="Z4" s="28">
+      <c r="N4" s="23"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="25"/>
+      <c r="Z4" s="18">
         <v>0.05</v>
       </c>
     </row>
@@ -10805,19 +10817,19 @@
         <v>42</v>
       </c>
       <c r="E5" s="11">
-        <f>C5*D5*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>44.1</v>
       </c>
-      <c r="N5" s="20"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="22"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="25"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
@@ -10833,19 +10845,19 @@
         <v>73</v>
       </c>
       <c r="E6" s="11">
-        <f>C6*D6*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>76.650000000000006</v>
       </c>
-      <c r="N6" s="20"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="22"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="25"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -10861,19 +10873,19 @@
         <v>46</v>
       </c>
       <c r="E7" s="11">
-        <f>C7*D7*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>96.600000000000009</v>
       </c>
-      <c r="N7" s="20"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="22"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="25"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -10889,19 +10901,19 @@
         <v>50</v>
       </c>
       <c r="E8" s="11">
-        <f>C8*D8*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
-      <c r="N8" s="20"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="22"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="25"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
@@ -10917,19 +10929,19 @@
         <v>77</v>
       </c>
       <c r="E9" s="11">
-        <f>C9*D9*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>161.70000000000002</v>
       </c>
-      <c r="N9" s="20"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="22"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="25"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
@@ -10945,19 +10957,19 @@
         <v>19</v>
       </c>
       <c r="E10" s="11">
-        <f>C10*D10*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>39.9</v>
       </c>
-      <c r="N10" s="20"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="22"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="25"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
@@ -10973,19 +10985,19 @@
         <v>44</v>
       </c>
       <c r="E11" s="11">
-        <f>C11*D11*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>46.2</v>
       </c>
-      <c r="N11" s="20"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="22"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="25"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
@@ -11001,19 +11013,19 @@
         <v>47</v>
       </c>
       <c r="E12" s="11">
-        <f>C12*D12*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>246.75</v>
       </c>
-      <c r="N12" s="20"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="22"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="25"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
@@ -11029,19 +11041,19 @@
         <v>3</v>
       </c>
       <c r="E13" s="11">
-        <f>C13*D13*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>12.600000000000001</v>
       </c>
-      <c r="N13" s="20"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="22"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="25"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
@@ -11057,19 +11069,19 @@
         <v>32</v>
       </c>
       <c r="E14" s="11">
-        <f>C14*D14*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>168</v>
       </c>
-      <c r="N14" s="20"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="22"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="25"/>
     </row>
     <row r="15" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
@@ -11085,19 +11097,19 @@
         <v>77</v>
       </c>
       <c r="E15" s="11">
-        <f>C15*D15*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>80.850000000000009</v>
       </c>
-      <c r="N15" s="23"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="25"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="28"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
@@ -11113,7 +11125,7 @@
         <v>39</v>
       </c>
       <c r="E16" s="11">
-        <f>C16*D16*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>122.85000000000001</v>
       </c>
     </row>
@@ -11131,7 +11143,7 @@
         <v>21</v>
       </c>
       <c r="E17" s="11">
-        <f>C17*D17*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>66.150000000000006</v>
       </c>
     </row>
@@ -11149,7 +11161,7 @@
         <v>65</v>
       </c>
       <c r="E18" s="11">
-        <f>C18*D18*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>68.25</v>
       </c>
     </row>
@@ -11167,7 +11179,7 @@
         <v>21</v>
       </c>
       <c r="E19" s="11">
-        <f>C19*D19*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>88.2</v>
       </c>
     </row>
@@ -11185,7 +11197,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="11">
-        <f>C20*D20*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>115.5</v>
       </c>
     </row>
@@ -11203,7 +11215,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="11">
-        <f>C21*D21*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
@@ -11505,35 +11517,41 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67CCA7B-0EC3-44B5-A412-5CDF79AC63E9}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="17" t="s">
         <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>16</v>
       </c>
@@ -11547,11 +11565,11 @@
         <v>26</v>
       </c>
       <c r="E2" s="11">
-        <f>C2*D2*(1+$Z$4)</f>
+        <f t="shared" ref="E2:E11" si="0">C2*D2*(1+$Z$4)</f>
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>15</v>
       </c>
@@ -11565,11 +11583,11 @@
         <v>69</v>
       </c>
       <c r="E3" s="11">
-        <f>C3*D3*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>10</v>
       </c>
@@ -11583,11 +11601,11 @@
         <v>3</v>
       </c>
       <c r="E4" s="11">
-        <f>C4*D4*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>6</v>
       </c>
@@ -11601,11 +11619,11 @@
         <v>42</v>
       </c>
       <c r="E5" s="11">
-        <f>C5*D5*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>9</v>
       </c>
@@ -11619,11 +11637,11 @@
         <v>73</v>
       </c>
       <c r="E6" s="11">
-        <f>C6*D6*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>14</v>
       </c>
@@ -11637,11 +11655,11 @@
         <v>46</v>
       </c>
       <c r="E7" s="11">
-        <f>C7*D7*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>24</v>
       </c>
@@ -11655,11 +11673,11 @@
         <v>50</v>
       </c>
       <c r="E8" s="11">
-        <f>C8*D8*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -11673,11 +11691,11 @@
         <v>77</v>
       </c>
       <c r="E9" s="11">
-        <f>C9*D9*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>22</v>
       </c>
@@ -11691,11 +11709,11 @@
         <v>19</v>
       </c>
       <c r="E10" s="11">
-        <f>C10*D10*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>14</v>
       </c>
@@ -11709,18 +11727,18 @@
         <v>44</v>
       </c>
       <c r="E11" s="11">
-        <f>C11*D11*(1+$Z$4)</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>5</v>
       </c>
@@ -11734,11 +11752,11 @@
         <v>3</v>
       </c>
       <c r="E13" s="11">
-        <f>C13*D13*(1+$Z$4)</f>
+        <f t="shared" ref="E13:E21" si="1">C13*D13*(1+$Z$4)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>27</v>
       </c>
@@ -11752,11 +11770,11 @@
         <v>32</v>
       </c>
       <c r="E14" s="11">
-        <f>C14*D14*(1+$Z$4)</f>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>22</v>
       </c>
@@ -11770,11 +11788,11 @@
         <v>77</v>
       </c>
       <c r="E15" s="11">
-        <f>C15*D15*(1+$Z$4)</f>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>2</v>
       </c>
@@ -11788,7 +11806,7 @@
         <v>39</v>
       </c>
       <c r="E16" s="11">
-        <f>C16*D16*(1+$Z$4)</f>
+        <f t="shared" si="1"/>
         <v>117</v>
       </c>
     </row>
@@ -11806,7 +11824,7 @@
         <v>21</v>
       </c>
       <c r="E17" s="11">
-        <f>C17*D17*(1+$Z$4)</f>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
     </row>
@@ -11824,7 +11842,7 @@
         <v>65</v>
       </c>
       <c r="E18" s="11">
-        <f>C18*D18*(1+$Z$4)</f>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
     </row>
@@ -11842,7 +11860,7 @@
         <v>21</v>
       </c>
       <c r="E19" s="11">
-        <f>C19*D19*(1+$Z$4)</f>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
@@ -11860,7 +11878,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="11">
-        <f>C20*D20*(1+$Z$4)</f>
+        <f t="shared" si="1"/>
         <v>110</v>
       </c>
     </row>
@@ -11878,7 +11896,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="11">
-        <f>C21*D21*(1+$Z$4)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>

</xml_diff>